<commit_message>
tuesday in-depth code review
</commit_message>
<xml_diff>
--- a/data/redd_counts.xlsx
+++ b/data/redd_counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/david_dayan_fws_gov/Documents/Documents/Bull Trout/yakima/Rimrock-Drawdown/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="13_ncr:40009_{1357F781-9F2A-426C-BAF3-03EDA5460B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{857F545C-0E69-4C16-B724-8292E9D83C10}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="13_ncr:40009_{1357F781-9F2A-426C-BAF3-03EDA5460B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A58E5C8B-3316-478E-AEC3-6E49D3ABE7C9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1485" windowWidth="21600" windowHeight="12630" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="redd_counts_raw" sheetId="1" r:id="rId1"/>
@@ -1285,10 +1285,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1588,7 +1584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
@@ -5041,8 +5037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:W89"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10:Q114"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5433,7 +5429,9 @@
       <c r="H30" s="2">
         <v>2014</v>
       </c>
-      <c r="I30" s="2"/>
+      <c r="I30" s="2">
+        <v>2018</v>
+      </c>
       <c r="J30" s="2"/>
       <c r="K30" s="19"/>
       <c r="L30" s="16"/>
@@ -6033,8 +6031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE016868-95F5-405A-8CA3-0AFB4F535522}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:B34"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>